<commit_message>
Updates in June and July 2014
Lots of updates to the scripts and datafiles.  These changes will be
documented elsewhere
</commit_message>
<xml_diff>
--- a/Tools/Tables/Tobler002.xlsx
+++ b/Tools/Tables/Tobler002.xlsx
@@ -4,18 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="24675" windowHeight="12555"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="24675" windowHeight="12555" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tobler002" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Biking-Maybe" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -844,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2308,7 +2305,7 @@
   <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4669,4 +4666,793 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A91" sqref="A1:B91"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>-45</v>
+      </c>
+      <c r="B1">
+        <f>1/COS((A1*1.4)/180*PI())</f>
+        <v>2.2026892645852665</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-44</v>
+      </c>
+      <c r="B2">
+        <f>1/COS((A2*1.4)/180*PI())</f>
+        <v>2.1025002111535627</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-43</v>
+      </c>
+      <c r="B3">
+        <f>1/COS((A3*1.4)/180*PI())</f>
+        <v>2.0121778572309417</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-42</v>
+      </c>
+      <c r="B4">
+        <f>1/COS((A4*1.4)/180*PI())</f>
+        <v>1.9304012762000771</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-41</v>
+      </c>
+      <c r="B5">
+        <f>1/COS((A5*1.4)/180*PI())</f>
+        <v>1.8560768843233801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-40</v>
+      </c>
+      <c r="B6">
+        <f>1/COS((A6*1.4)/180*PI())</f>
+        <v>1.7882916499714008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-39</v>
+      </c>
+      <c r="B7">
+        <f>1/COS((A7*1.4)/180*PI())</f>
+        <v>1.7262774068003734</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-38</v>
+      </c>
+      <c r="B8">
+        <f>1/COS((A8*1.4)/180*PI())</f>
+        <v>1.6693833139095957</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-37</v>
+      </c>
+      <c r="B9">
+        <f>1/COS((A9*1.4)/180*PI())</f>
+        <v>1.6170543729792275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-36</v>
+      </c>
+      <c r="B10">
+        <f>1/COS((A10*1.4)/180*PI())</f>
+        <v>1.5688145035053653</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-35</v>
+      </c>
+      <c r="B11">
+        <f>1/COS((A11*1.4)/180*PI())</f>
+        <v>1.5242530867058139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-34</v>
+      </c>
+      <c r="B12">
+        <f>1/COS((A12*1.4)/180*PI())</f>
+        <v>1.4830141764488962</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-33</v>
+      </c>
+      <c r="B13">
+        <f>1/COS((A13*1.4)/180*PI())</f>
+        <v>1.4447877805513611</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-32</v>
+      </c>
+      <c r="B14">
+        <f>1/COS((A14*1.4)/180*PI())</f>
+        <v>1.4093027636414244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-31</v>
+      </c>
+      <c r="B15">
+        <f>1/COS((A15*1.4)/180*PI())</f>
+        <v>1.3763210306569391</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-30</v>
+      </c>
+      <c r="B16">
+        <f>1/COS((A16*1.4)/180*PI())</f>
+        <v>1.3456327296063761</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-29</v>
+      </c>
+      <c r="B17">
+        <f>1/COS((A17*1.4)/180*PI())</f>
+        <v>1.3170522714865931</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-28</v>
+      </c>
+      <c r="B18">
+        <f>1/COS((A18*1.4)/180*PI())</f>
+        <v>1.2904150098185045</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-27</v>
+      </c>
+      <c r="B19">
+        <f>1/COS((A19*1.4)/180*PI())</f>
+        <v>1.2655744560720901</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-26</v>
+      </c>
+      <c r="B20">
+        <f>1/COS((A20*1.4)/180*PI())</f>
+        <v>1.2423999331154147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-25</v>
+      </c>
+      <c r="B21">
+        <f>1/COS((A21*1.4)/180*PI())</f>
+        <v>1.2207745887614561</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-24</v>
+      </c>
+      <c r="B22">
+        <f>1/COS((A22*1.4)/180*PI())</f>
+        <v>1.200593706972173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>-23</v>
+      </c>
+      <c r="B23">
+        <f>1/COS((A23*1.4)/180*PI())</f>
+        <v>1.1817632663902291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-22</v>
+      </c>
+      <c r="B24">
+        <f>1/COS((A24*1.4)/180*PI())</f>
+        <v>1.1641987054032632</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-21</v>
+      </c>
+      <c r="B25">
+        <f>1/COS((A25*1.4)/180*PI())</f>
+        <v>1.1478238604989741</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>-20</v>
+      </c>
+      <c r="B26">
+        <f>1/COS((A26*1.4)/180*PI())</f>
+        <v>1.132570050689039</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-19</v>
+      </c>
+      <c r="B27">
+        <f>1/COS((A27*1.4)/180*PI())</f>
+        <v>1.118375285604833</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>-18</v>
+      </c>
+      <c r="B28">
+        <f>1/COS((A28*1.4)/180*PI())</f>
+        <v>1.1051835787563995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>-17</v>
+      </c>
+      <c r="B29">
+        <f>1/COS((A29*1.4)/180*PI())</f>
+        <v>1.092944350596373</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>-16</v>
+      </c>
+      <c r="B30">
+        <f>1/COS((A30*1.4)/180*PI())</f>
+        <v>1.0816119085957019</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>-15</v>
+      </c>
+      <c r="B31">
+        <f>1/COS((A31*1.4)/180*PI())</f>
+        <v>1.071144993637029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>-14</v>
+      </c>
+      <c r="B32">
+        <f>1/COS((A32*1.4)/180*PI())</f>
+        <v>1.0615063837574521</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>-13</v>
+      </c>
+      <c r="B33">
+        <f>1/COS((A33*1.4)/180*PI())</f>
+        <v>1.0526625476981721</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-12</v>
+      </c>
+      <c r="B34">
+        <f>1/COS((A34*1.4)/180*PI())</f>
+        <v>1.0445833419020103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>-11</v>
+      </c>
+      <c r="B35">
+        <f>1/COS((A35*1.4)/180*PI())</f>
+        <v>1.0372417455868002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>-10</v>
+      </c>
+      <c r="B36">
+        <f>1/COS((A36*1.4)/180*PI())</f>
+        <v>1.0306136293498982</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>-9</v>
+      </c>
+      <c r="B37">
+        <f>1/COS((A37*1.4)/180*PI())</f>
+        <v>1.0246775534559003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>-8</v>
+      </c>
+      <c r="B38">
+        <f>1/COS((A38*1.4)/180*PI())</f>
+        <v>1.0194145925498797</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>-7</v>
+      </c>
+      <c r="B39">
+        <f>1/COS((A39*1.4)/180*PI())</f>
+        <v>1.0148081840413159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>-6</v>
+      </c>
+      <c r="B40">
+        <f>1/COS((A40*1.4)/180*PI())</f>
+        <v>1.0108439978351371</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>-5</v>
+      </c>
+      <c r="B41">
+        <f>1/COS((A41*1.4)/180*PI())</f>
+        <v>1.0075098254588484</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>-4</v>
+      </c>
+      <c r="B42">
+        <f>1/COS((A42*1.4)/180*PI())</f>
+        <v>1.0047954869593181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>-3</v>
+      </c>
+      <c r="B43">
+        <f>1/COS((A43*1.4)/180*PI())</f>
+        <v>1.002692754228351</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>-2</v>
+      </c>
+      <c r="B44">
+        <f>1/COS((A44*1.4)/180*PI())</f>
+        <v>1.0011952896702694</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>-1</v>
+      </c>
+      <c r="B45">
+        <f>1/COS((A45*1.4)/180*PI())</f>
+        <v>1.0002985993537754</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <f>1/COS((A46*1.4)/180*PI())</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>0.94073600387004974</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>0.88495127390790829</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>0.83241245027661315</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>0.78290506010728989</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>0.73623175718467948</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>6</v>
+      </c>
+      <c r="B52">
+        <v>0.69221074603919241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>7</v>
+      </c>
+      <c r="B53">
+        <v>0.65067436899001063</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>8</v>
+      </c>
+      <c r="B54">
+        <v>0.61146783741132915</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <v>0.57444809084553139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56">
+        <v>0.53948276961858599</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>11</v>
+      </c>
+      <c r="B57">
+        <v>0.50644928837105219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>12</v>
+      </c>
+      <c r="B58">
+        <v>0.47523399944234646</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>13</v>
+      </c>
+      <c r="B59">
+        <v>0.44573143636977447</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>14</v>
+      </c>
+      <c r="B60">
+        <v>0.41784362891561178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>15</v>
+      </c>
+      <c r="B61">
+        <v>0.39147948203925742</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>16</v>
+      </c>
+      <c r="B62">
+        <v>0.3665542121076944</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>17</v>
+      </c>
+      <c r="B63">
+        <v>0.34298883440357325</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>18</v>
+      </c>
+      <c r="B64">
+        <v>0.32070969666113225</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>19</v>
+      </c>
+      <c r="B65">
+        <v>0.29964805394860622</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>20</v>
+      </c>
+      <c r="B66">
+        <v>0.27973968073271621</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>21</v>
+      </c>
+      <c r="B67">
+        <v>0.26092451641563863</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>22</v>
+      </c>
+      <c r="B68">
+        <v>0.24314634103564536</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>23</v>
+      </c>
+      <c r="B69">
+        <v>0.22635247817633528</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>24</v>
+      </c>
+      <c r="B70">
+        <v>0.21049352244206965</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>25</v>
+      </c>
+      <c r="B71">
+        <v>0.19552308913412081</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>26</v>
+      </c>
+      <c r="B72">
+        <v>0.18139758400764319</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>27</v>
+      </c>
+      <c r="B73">
+        <v>0.16807599120784555</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>28</v>
+      </c>
+      <c r="B74">
+        <v>0.15551967767810956</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>29</v>
+      </c>
+      <c r="B75">
+        <v>0.14369221250627179</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>30</v>
+      </c>
+      <c r="B76">
+        <v>0.13255919983050554</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>31</v>
+      </c>
+      <c r="B77">
+        <v>0.12208812406553485</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>32</v>
+      </c>
+      <c r="B78">
+        <v>0.11224820633533836</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>33</v>
+      </c>
+      <c r="B79">
+        <v>0.10301027111188625</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>34</v>
+      </c>
+      <c r="B80">
+        <v>9.4346622162437235E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>35</v>
+      </c>
+      <c r="B81">
+        <v>8.6230927001965163E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>36</v>
+      </c>
+      <c r="B82">
+        <v>7.8638109133720629E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>37</v>
+      </c>
+      <c r="B83">
+        <v>7.1544247440966477E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>38</v>
+      </c>
+      <c r="B84">
+        <v>6.4926482167656313E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>39</v>
+      </c>
+      <c r="B85">
+        <v>5.8762926996282092E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>40</v>
+      </c>
+      <c r="B86">
+        <v>5.3032586798219997E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>41</v>
+      </c>
+      <c r="B87">
+        <v>4.7715280696534246E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>42</v>
+      </c>
+      <c r="B88">
+        <v>4.2791570144141346E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>43</v>
+      </c>
+      <c r="B89">
+        <v>3.8242691782221956E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>44</v>
+      </c>
+      <c r="B90">
+        <v>3.4050494905427824E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>45</v>
+      </c>
+      <c r="B91">
+        <v>3.0197383422318508E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>